<commit_message>
Add HeStore basket only for boards
</commit_message>
<xml_diff>
--- a/PCB_design/Board sizes.xlsx
+++ b/PCB_design/Board sizes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="f:\Dokumentumok\Dev\Arduino\RGB_Controller\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="f:\Dokumentumok\Dev\Arduino\RGB-Controller\PCB_design\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>inch</t>
   </si>
@@ -36,6 +36,12 @@
   </si>
   <si>
     <t>Pot panel</t>
+  </si>
+  <si>
+    <t>Pot</t>
+  </si>
+  <si>
+    <t>RGB</t>
   </si>
 </sst>
 </file>
@@ -52,15 +58,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -68,15 +80,160 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -358,73 +515,381 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C6"/>
+  <dimension ref="A2:V18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" style="2" customWidth="1"/>
+    <col min="2" max="4" width="9.140625" style="2"/>
+    <col min="5" max="129" width="2.85546875" style="2" customWidth="1"/>
+    <col min="130" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="2" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="3">
         <v>3</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="3">
         <f>B3*2.54</f>
         <v>7.62</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="1">
+      <c r="E3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M3" s="7"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4"/>
+      <c r="U3" s="4"/>
+      <c r="V3" s="4"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="3">
         <v>2.5499999999999998</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="3">
         <f t="shared" ref="C4:C6" si="0">B4*2.54</f>
         <v>6.4769999999999994</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="E4" s="9"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
+      <c r="U4" s="4"/>
+      <c r="V4" s="4"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>1.55</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="3">
         <f t="shared" si="0"/>
         <v>3.9370000000000003</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6">
+      <c r="E5" s="9"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
+      <c r="U5" s="4"/>
+      <c r="V5" s="4"/>
+    </row>
+    <row r="6" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="2">
         <v>1</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="3">
         <f t="shared" si="0"/>
         <v>2.54</v>
       </c>
+      <c r="E6" s="9"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4"/>
+      <c r="S6" s="4"/>
+      <c r="T6" s="4"/>
+      <c r="U6" s="4"/>
+      <c r="V6" s="4"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E7" s="9"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
+      <c r="S7" s="4"/>
+      <c r="T7" s="4"/>
+      <c r="U7" s="4"/>
+      <c r="V7" s="4"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E8" s="9"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="4"/>
+      <c r="U8" s="4"/>
+      <c r="V8" s="4"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E9" s="9"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="4"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="4"/>
+      <c r="U9" s="4"/>
+      <c r="V9" s="4"/>
+    </row>
+    <row r="10" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E10" s="12"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="4"/>
+      <c r="S10" s="4"/>
+      <c r="T10" s="4"/>
+      <c r="U10" s="4"/>
+      <c r="V10" s="4"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E11" s="21"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="4"/>
+      <c r="S11" s="4"/>
+      <c r="T11" s="4"/>
+      <c r="U11" s="4"/>
+      <c r="V11" s="4"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E12" s="17"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4"/>
+      <c r="S12" s="4"/>
+      <c r="T12" s="4"/>
+      <c r="U12" s="4"/>
+      <c r="V12" s="4"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E13" s="17"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="4"/>
+      <c r="S13" s="4"/>
+      <c r="T13" s="4"/>
+      <c r="U13" s="4"/>
+      <c r="V13" s="4"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E14" s="17"/>
+      <c r="F14" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="4"/>
+      <c r="S14" s="4"/>
+      <c r="T14" s="4"/>
+      <c r="U14" s="4"/>
+      <c r="V14" s="4"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E15" s="17"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="15"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="4"/>
+      <c r="R15" s="4"/>
+      <c r="S15" s="4"/>
+      <c r="T15" s="4"/>
+      <c r="U15" s="4"/>
+      <c r="V15" s="4"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E16" s="17"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="15"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="4"/>
+      <c r="R16" s="4"/>
+      <c r="S16" s="4"/>
+      <c r="T16" s="4"/>
+      <c r="U16" s="4"/>
+      <c r="V16" s="4"/>
+    </row>
+    <row r="17" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E17" s="17"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="15"/>
+      <c r="N17" s="16"/>
+    </row>
+    <row r="18" spans="5:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E18" s="18"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="19"/>
+      <c r="N18" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="5">
+    <mergeCell ref="F14:J14"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="A5:A6"/>
+    <mergeCell ref="L3:N6"/>
+    <mergeCell ref="E3:K10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Update PCB for using arduino nano
</commit_message>
<xml_diff>
--- a/PCB_design/Board sizes.xlsx
+++ b/PCB_design/Board sizes.xlsx
@@ -167,19 +167,49 @@
   <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -193,9 +223,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -207,33 +234,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -518,370 +518,370 @@
   <dimension ref="A2:V18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T4" sqref="T4"/>
+      <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" style="2" customWidth="1"/>
-    <col min="2" max="4" width="9.140625" style="2"/>
-    <col min="5" max="129" width="2.85546875" style="2" customWidth="1"/>
-    <col min="130" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="18.7109375" style="1" customWidth="1"/>
+    <col min="2" max="4" width="9.140625" style="1"/>
+    <col min="5" max="129" width="2.85546875" style="1" customWidth="1"/>
+    <col min="130" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>3</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <f>B3*2.54</f>
         <v>7.62</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="6" t="s">
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="7"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
-      <c r="T3" s="4"/>
-      <c r="U3" s="4"/>
-      <c r="V3" s="4"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="3">
-        <v>2.5499999999999998</v>
-      </c>
-      <c r="C4" s="3">
+      <c r="A4" s="15"/>
+      <c r="B4" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="C4" s="2">
         <f t="shared" ref="C4:C6" si="0">B4*2.54</f>
-        <v>6.4769999999999994</v>
-      </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
-      <c r="S4" s="4"/>
-      <c r="T4" s="4"/>
-      <c r="U4" s="4"/>
-      <c r="V4" s="4"/>
+        <v>6.35</v>
+      </c>
+      <c r="E4" s="19"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>1.55</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <f t="shared" si="0"/>
         <v>3.9370000000000003</v>
       </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="11"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="4"/>
-      <c r="S5" s="4"/>
-      <c r="T5" s="4"/>
-      <c r="U5" s="4"/>
-      <c r="V5" s="4"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="20"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
     </row>
     <row r="6" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
-      <c r="B6" s="2">
+      <c r="A6" s="15"/>
+      <c r="B6" s="1">
         <v>1</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <f t="shared" si="0"/>
         <v>2.54</v>
       </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
-      <c r="S6" s="4"/>
-      <c r="T6" s="4"/>
-      <c r="U6" s="4"/>
-      <c r="V6" s="4"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="21"/>
+      <c r="M6" s="22"/>
+      <c r="N6" s="23"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="E7" s="9"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="15"/>
-      <c r="N7" s="16"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="4"/>
-      <c r="S7" s="4"/>
-      <c r="T7" s="4"/>
-      <c r="U7" s="4"/>
-      <c r="V7" s="4"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="E8" s="9"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="16"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="4"/>
-      <c r="S8" s="4"/>
-      <c r="T8" s="4"/>
-      <c r="U8" s="4"/>
-      <c r="V8" s="4"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="E9" s="9"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="15"/>
-      <c r="N9" s="16"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="4"/>
-      <c r="R9" s="4"/>
-      <c r="S9" s="4"/>
-      <c r="T9" s="4"/>
-      <c r="U9" s="4"/>
-      <c r="V9" s="4"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="3"/>
+      <c r="V9" s="3"/>
     </row>
     <row r="10" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E10" s="12"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="15"/>
-      <c r="N10" s="16"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="4"/>
-      <c r="Q10" s="4"/>
-      <c r="R10" s="4"/>
-      <c r="S10" s="4"/>
-      <c r="T10" s="4"/>
-      <c r="U10" s="4"/>
-      <c r="V10" s="4"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+      <c r="T10" s="3"/>
+      <c r="U10" s="3"/>
+      <c r="V10" s="3"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="E11" s="21"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="22"/>
-      <c r="K11" s="23"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="16"/>
-      <c r="O11" s="5"/>
-      <c r="P11" s="4"/>
-      <c r="Q11" s="4"/>
-      <c r="R11" s="4"/>
-      <c r="S11" s="4"/>
-      <c r="T11" s="4"/>
-      <c r="U11" s="4"/>
-      <c r="V11" s="4"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+      <c r="T11" s="3"/>
+      <c r="U11" s="3"/>
+      <c r="V11" s="3"/>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="E12" s="17"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="16"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="15"/>
-      <c r="N12" s="16"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="4"/>
-      <c r="Q12" s="4"/>
-      <c r="R12" s="4"/>
-      <c r="S12" s="4"/>
-      <c r="T12" s="4"/>
-      <c r="U12" s="4"/>
-      <c r="V12" s="4"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
+      <c r="T12" s="3"/>
+      <c r="U12" s="3"/>
+      <c r="V12" s="3"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="E13" s="17"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="16"/>
-      <c r="L13" s="15"/>
-      <c r="M13" s="15"/>
-      <c r="N13" s="16"/>
-      <c r="O13" s="5"/>
-      <c r="P13" s="4"/>
-      <c r="Q13" s="4"/>
-      <c r="R13" s="4"/>
-      <c r="S13" s="4"/>
-      <c r="T13" s="4"/>
-      <c r="U13" s="4"/>
-      <c r="V13" s="4"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
+      <c r="T13" s="3"/>
+      <c r="U13" s="3"/>
+      <c r="V13" s="3"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="E14" s="17"/>
-      <c r="F14" s="10" t="s">
+      <c r="E14" s="7"/>
+      <c r="F14" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="16"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="16"/>
-      <c r="O14" s="5"/>
-      <c r="P14" s="4"/>
-      <c r="Q14" s="4"/>
-      <c r="R14" s="4"/>
-      <c r="S14" s="4"/>
-      <c r="T14" s="4"/>
-      <c r="U14" s="4"/>
-      <c r="V14" s="4"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="3"/>
+      <c r="T14" s="3"/>
+      <c r="U14" s="3"/>
+      <c r="V14" s="3"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="E15" s="17"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="16"/>
-      <c r="L15" s="15"/>
-      <c r="M15" s="15"/>
-      <c r="N15" s="16"/>
-      <c r="O15" s="5"/>
-      <c r="P15" s="4"/>
-      <c r="Q15" s="4"/>
-      <c r="R15" s="4"/>
-      <c r="S15" s="4"/>
-      <c r="T15" s="4"/>
-      <c r="U15" s="4"/>
-      <c r="V15" s="4"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="3"/>
+      <c r="T15" s="3"/>
+      <c r="U15" s="3"/>
+      <c r="V15" s="3"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="E16" s="17"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="16"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="15"/>
-      <c r="N16" s="16"/>
-      <c r="O16" s="5"/>
-      <c r="P16" s="4"/>
-      <c r="Q16" s="4"/>
-      <c r="R16" s="4"/>
-      <c r="S16" s="4"/>
-      <c r="T16" s="4"/>
-      <c r="U16" s="4"/>
-      <c r="V16" s="4"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+      <c r="S16" s="3"/>
+      <c r="T16" s="3"/>
+      <c r="U16" s="3"/>
+      <c r="V16" s="3"/>
     </row>
     <row r="17" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="E17" s="17"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="16"/>
-      <c r="L17" s="15"/>
-      <c r="M17" s="15"/>
-      <c r="N17" s="16"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="6"/>
     </row>
     <row r="18" spans="5:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E18" s="18"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="20"/>
-      <c r="L18" s="19"/>
-      <c r="M18" s="19"/>
-      <c r="N18" s="20"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>